<commit_message>
Input sheet data clean, readme notes
</commit_message>
<xml_diff>
--- a/api/order/sample_sheets/sample-order-v070420.xlsx
+++ b/api/order/sample_sheets/sample-order-v070420.xlsx
@@ -94,13 +94,13 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Collection</t>
+    <t xml:space="preserve">COLLECTION</t>
   </si>
   <si>
     <t xml:space="preserve">If collection, please state which shop: (Ockley/Denbies)</t>
   </si>
   <si>
-    <t xml:space="preserve">Denbies</t>
+    <t xml:space="preserve">dENBIES</t>
   </si>
   <si>
     <t xml:space="preserve">Deliver / Collection Date</t>
@@ -929,9 +929,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2293200</xdr:colOff>
+      <xdr:colOff>2292480</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>635760</xdr:rowOff>
+      <xdr:rowOff>635040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -945,7 +945,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5307840" y="9360"/>
-          <a:ext cx="816840" cy="626400"/>
+          <a:ext cx="816120" cy="625680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -967,8 +967,8 @@
   </sheetPr>
   <dimension ref="A1:Z84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>